<commit_message>
add 116th congress house members
</commit_message>
<xml_diff>
--- a/hannah/house_committees.xlsx
+++ b/hannah/house_committees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b82b5f88a6e55c46/School/University of Waterloo ^0 Wilfrid Laurier University/4B Spring 2021/BU 493Y/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bu493-project\hannah\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{CBA01935-AD88-4125-BD6F-A09BA0276FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{905538B1-10E9-487E-8A61-750A31D61AE0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0E10E9-8635-4635-B545-DF72CB121ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36560" yWindow="3660" windowWidth="20770" windowHeight="12580" xr2:uid="{26F9241C-1752-4336-BA30-13A2D78619E4}"/>
+    <workbookView xWindow="-22740" yWindow="5460" windowWidth="20770" windowHeight="12580" xr2:uid="{26F9241C-1752-4336-BA30-13A2D78619E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3360" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3424" uniqueCount="535">
   <si>
     <t>Appropriations</t>
   </si>
@@ -1640,6 +1640,54 @@
   </si>
   <si>
     <t>Committee</t>
+  </si>
+  <si>
+    <t>Greg Gianforte</t>
+  </si>
+  <si>
+    <t>Joe Kennedy III</t>
+  </si>
+  <si>
+    <t>Gil Cisneros</t>
+  </si>
+  <si>
+    <t>George Holding</t>
+  </si>
+  <si>
+    <t>Susan Davis</t>
+  </si>
+  <si>
+    <t>Pete Visclosky</t>
+  </si>
+  <si>
+    <t>Francis Rooney</t>
+  </si>
+  <si>
+    <t>Justin Amash</t>
+  </si>
+  <si>
+    <t>Donna Shalala</t>
+  </si>
+  <si>
+    <t>Susan Brooks</t>
+  </si>
+  <si>
+    <t>Roger Marshall</t>
+  </si>
+  <si>
+    <t>Harley Rouda</t>
+  </si>
+  <si>
+    <t>Phil Roe</t>
+  </si>
+  <si>
+    <t>Lacy Clay</t>
+  </si>
+  <si>
+    <t>Kenny Marchant</t>
+  </si>
+  <si>
+    <t>Mike Conaway</t>
   </si>
 </sst>
 </file>
@@ -2027,10 +2075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA51BD1F-BBF9-449B-BDA9-27B306C87E81}">
-  <dimension ref="A1:D839"/>
+  <dimension ref="A1:D871"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A828" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E836" sqref="E836"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14623,6 +14671,358 @@
       </c>
       <c r="D839">
         <v>117</v>
+      </c>
+    </row>
+    <row r="840" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B840" t="s">
+        <v>519</v>
+      </c>
+      <c r="C840" t="s">
+        <v>400</v>
+      </c>
+      <c r="D840">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="841" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B841" t="s">
+        <v>519</v>
+      </c>
+      <c r="C841" t="s">
+        <v>425</v>
+      </c>
+      <c r="D841">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="842" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B842" t="s">
+        <v>520</v>
+      </c>
+      <c r="C842" t="s">
+        <v>225</v>
+      </c>
+      <c r="D842">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="843" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B843" t="s">
+        <v>521</v>
+      </c>
+      <c r="C843" t="s">
+        <v>1</v>
+      </c>
+      <c r="D843">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="844" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B844" t="s">
+        <v>521</v>
+      </c>
+      <c r="C844" t="s">
+        <v>478</v>
+      </c>
+      <c r="D844">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="845" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B845" t="s">
+        <v>522</v>
+      </c>
+      <c r="C845" t="s">
+        <v>484</v>
+      </c>
+      <c r="D845">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="846" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B846" t="s">
+        <v>522</v>
+      </c>
+      <c r="C846" t="s">
+        <v>2</v>
+      </c>
+      <c r="D846">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="847" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B847" t="s">
+        <v>522</v>
+      </c>
+      <c r="C847" t="s">
+        <v>273</v>
+      </c>
+      <c r="D847">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="848" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B848" t="s">
+        <v>534</v>
+      </c>
+      <c r="C848" t="s">
+        <v>33</v>
+      </c>
+      <c r="D848">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="849" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B849" t="s">
+        <v>534</v>
+      </c>
+      <c r="C849" t="s">
+        <v>1</v>
+      </c>
+      <c r="D849">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="850" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B850" t="s">
+        <v>523</v>
+      </c>
+      <c r="C850" t="s">
+        <v>224</v>
+      </c>
+      <c r="D850">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="851" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B851" t="s">
+        <v>523</v>
+      </c>
+      <c r="C851" t="s">
+        <v>1</v>
+      </c>
+      <c r="D851">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="852" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B852" t="s">
+        <v>523</v>
+      </c>
+      <c r="C852" t="s">
+        <v>377</v>
+      </c>
+      <c r="D852">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="853" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B853" t="s">
+        <v>524</v>
+      </c>
+      <c r="C853" t="s">
+        <v>0</v>
+      </c>
+      <c r="D853">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="854" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B854" t="s">
+        <v>525</v>
+      </c>
+      <c r="C854" t="s">
+        <v>224</v>
+      </c>
+      <c r="D854">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="855" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B855" t="s">
+        <v>525</v>
+      </c>
+      <c r="C855" t="s">
+        <v>358</v>
+      </c>
+      <c r="D855">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="856" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B856" t="s">
+        <v>526</v>
+      </c>
+      <c r="C856" t="s">
+        <v>425</v>
+      </c>
+      <c r="D856">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="857" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B857" t="s">
+        <v>527</v>
+      </c>
+      <c r="C857" t="s">
+        <v>224</v>
+      </c>
+      <c r="D857">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="858" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B858" t="s">
+        <v>527</v>
+      </c>
+      <c r="C858" t="s">
+        <v>439</v>
+      </c>
+      <c r="D858">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="859" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B859" t="s">
+        <v>528</v>
+      </c>
+      <c r="C859" t="s">
+        <v>225</v>
+      </c>
+      <c r="D859">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="860" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B860" t="s">
+        <v>528</v>
+      </c>
+      <c r="C860" t="s">
+        <v>273</v>
+      </c>
+      <c r="D860">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="861" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B861" t="s">
+        <v>529</v>
+      </c>
+      <c r="C861" t="s">
+        <v>33</v>
+      </c>
+      <c r="D861">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="862" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B862" t="s">
+        <v>529</v>
+      </c>
+      <c r="C862" t="s">
+        <v>444</v>
+      </c>
+      <c r="D862">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="863" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B863" t="s">
+        <v>529</v>
+      </c>
+      <c r="C863" t="s">
+        <v>455</v>
+      </c>
+      <c r="D863">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="864" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B864" t="s">
+        <v>530</v>
+      </c>
+      <c r="C864" t="s">
+        <v>425</v>
+      </c>
+      <c r="D864">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="865" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B865" t="s">
+        <v>530</v>
+      </c>
+      <c r="C865" t="s">
+        <v>465</v>
+      </c>
+      <c r="D865">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="866" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B866" t="s">
+        <v>531</v>
+      </c>
+      <c r="C866" t="s">
+        <v>478</v>
+      </c>
+      <c r="D866">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="867" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B867" t="s">
+        <v>531</v>
+      </c>
+      <c r="C867" t="s">
+        <v>224</v>
+      </c>
+      <c r="D867">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="868" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B868" t="s">
+        <v>532</v>
+      </c>
+      <c r="C868" t="s">
+        <v>278</v>
+      </c>
+      <c r="D868">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="869" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B869" t="s">
+        <v>532</v>
+      </c>
+      <c r="C869" t="s">
+        <v>425</v>
+      </c>
+      <c r="D869">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="870" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B870" t="s">
+        <v>533</v>
+      </c>
+      <c r="C870" t="s">
+        <v>484</v>
+      </c>
+      <c r="D870">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="871" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B871" t="s">
+        <v>533</v>
+      </c>
+      <c r="C871" t="s">
+        <v>273</v>
+      </c>
+      <c r="D871">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -14993,6 +15393,7 @@
     <hyperlink ref="A839" r:id="rId364" tooltip="Carol Miller (politician)" display="https://en.wikipedia.org/wiki/Carol_Miller_(politician)" xr:uid="{B32328F0-1DB2-3A43-9755-F03704031A13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId365"/>
 </worksheet>
 </file>
 
@@ -15000,8 +15401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D87D28-1D94-4838-A592-11958C1D5783}">
   <dimension ref="A1:D839"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A814" workbookViewId="0">
+      <selection activeCell="B822" sqref="B822"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>